<commit_message>
Fixing all functions with limits
</commit_message>
<xml_diff>
--- a/setup/setup_Template.xlsx
+++ b/setup/setup_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f215465b21b5e6e2/Studium/34_Github/PyEVPowerKit/setup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{B7CA4536-B758-4683-983B-F8B7FD8E2847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF5CFEF9-BA6D-4571-87E7-D88B3CB676E1}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{B7CA4536-B758-4683-983B-F8B7FD8E2847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2B04806-6E13-495E-AE6C-B420B29EA686}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
@@ -1094,10 +1094,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1931,7 +1927,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2389,7 +2385,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2596,7 +2592,7 @@
         <v>1373</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3042,7 +3038,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A2:A37"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3288,7 +3284,7 @@
         <v>1373</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -3799,7 +3795,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3863,10 +3859,10 @@
         <v>292</v>
       </c>
       <c r="E3" s="11">
-        <v>1373</v>
+        <v>971</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>107</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>